<commit_message>
NA haver pull update
</commit_message>
<xml_diff>
--- a/development/features/spreadsheet-update/output/national_accounts.xlsx
+++ b/development/features/spreadsheet-update/output/national_accounts.xlsx
@@ -447,7 +447,7 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>21157.6</t>
+          <t>21157.1</t>
         </is>
       </c>
     </row>
@@ -536,12 +536,12 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>1599.3</t>
+          <t>1600.1</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>1686.4</t>
+          <t>1687.2</t>
         </is>
       </c>
     </row>
@@ -630,12 +630,12 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>1360.8</t>
+          <t>1369.2</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>1414.2</t>
+          <t>1429.6</t>
         </is>
       </c>
     </row>
@@ -682,7 +682,7 @@
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>193.9</t>
+          <t>205.3</t>
         </is>
       </c>
     </row>
@@ -729,7 +729,7 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>505.4</t>
+          <t>499.4</t>
         </is>
       </c>
     </row>
@@ -776,7 +776,7 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>1315.1</t>
+          <t>1317.3</t>
         </is>
       </c>
     </row>
@@ -882,42 +882,42 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>63.50000</t>
+          <t>63.5</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>68.50000</t>
+          <t>68.5</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>68.70000</t>
+          <t>68.7</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>69.80000</t>
+          <t>69.8</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>71.00000</t>
+          <t>71.0</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>62.70000</t>
+          <t>62.7</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>54.20000</t>
+          <t>54.2</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>62.63333</t>
+          <t>79.1</t>
         </is>
       </c>
     </row>
@@ -1075,7 +1075,7 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 771503</t>
+          <t xml:space="preserve"> 768678</t>
         </is>
       </c>
     </row>
@@ -1109,7 +1109,7 @@
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 56700</t>
+          <t xml:space="preserve"> 58400</t>
         </is>
       </c>
     </row>
@@ -1168,12 +1168,12 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>609.3</t>
+          <t>609300</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>865.6</t>
+          <t>865600</t>
         </is>
       </c>
     </row>
@@ -1185,12 +1185,12 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>63.8</t>
+          <t>63800</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>15.0</t>
+          <t>15000</t>
         </is>
       </c>
     </row>
@@ -1202,12 +1202,12 @@
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>73.3</t>
+          <t>73300</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>73.3</t>
+          <t>73300</t>
         </is>
       </c>
     </row>
@@ -1219,12 +1219,12 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>140</t>
+          <t>140000</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>140</t>
+          <t>140000</t>
         </is>
       </c>
     </row>
@@ -1318,7 +1318,7 @@
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>1486617</t>
+          <t>1486802</t>
         </is>
       </c>
     </row>
@@ -1365,7 +1365,7 @@
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>1335229</t>
+          <t>1335322</t>
         </is>
       </c>
     </row>
@@ -1459,7 +1459,7 @@
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>843592</t>
+          <t>835999</t>
         </is>
       </c>
     </row>
@@ -1506,7 +1506,7 @@
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>698983</t>
+          <t>691267</t>
         </is>
       </c>
     </row>
@@ -1553,7 +1553,7 @@
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>1996158</t>
+          <t>1992677</t>
         </is>
       </c>
     </row>
@@ -1600,7 +1600,7 @@
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>2337877</t>
+          <t>2329677</t>
         </is>
       </c>
     </row>
@@ -1681,7 +1681,7 @@
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 38500</t>
+          <t xml:space="preserve"> 39200</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
updated main spreadsheet with revised GDP
</commit_message>
<xml_diff>
--- a/development/features/spreadsheet-update/output/national_accounts.xlsx
+++ b/development/features/spreadsheet-update/output/national_accounts.xlsx
@@ -447,7 +447,7 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>21157.1</t>
+          <t>21170.3</t>
         </is>
       </c>
     </row>
@@ -494,7 +494,7 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>18583.5</t>
+          <t>18596.5</t>
         </is>
       </c>
     </row>
@@ -541,7 +541,7 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>1687.2</t>
+          <t>1687.4</t>
         </is>
       </c>
     </row>
@@ -635,7 +635,7 @@
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>1429.6</t>
+          <t>1430.2</t>
         </is>
       </c>
     </row>
@@ -682,7 +682,7 @@
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>205.3</t>
+          <t>207.0</t>
         </is>
       </c>
     </row>
@@ -729,7 +729,7 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>499.4</t>
+          <t>506.6</t>
         </is>
       </c>
     </row>
@@ -776,7 +776,7 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>1317.3</t>
+          <t>1344.5</t>
         </is>
       </c>
     </row>
@@ -870,7 +870,7 @@
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>12998</t>
+          <t>13001</t>
         </is>
       </c>
     </row>
@@ -917,7 +917,7 @@
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>79.1</t>
+          <t>90.2</t>
         </is>
       </c>
     </row>
@@ -964,7 +964,7 @@
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>3488125</t>
+          <t>3494888</t>
         </is>
       </c>
     </row>
@@ -1075,7 +1075,7 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 768678</t>
+          <t xml:space="preserve"> 775154</t>
         </is>
       </c>
     </row>
@@ -1156,7 +1156,7 @@
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>1213308</t>
+          <t>1213480</t>
         </is>
       </c>
     </row>
@@ -1318,7 +1318,7 @@
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>1486802</t>
+          <t>1487035</t>
         </is>
       </c>
     </row>
@@ -1365,7 +1365,7 @@
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>1335322</t>
+          <t>1335133</t>
         </is>
       </c>
     </row>
@@ -1459,7 +1459,7 @@
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>835999</t>
+          <t>828480</t>
         </is>
       </c>
     </row>
@@ -1506,7 +1506,7 @@
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>691267</t>
+          <t>683703</t>
         </is>
       </c>
     </row>
@@ -1553,7 +1553,7 @@
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>1992677</t>
+          <t>1993051</t>
         </is>
       </c>
     </row>
@@ -1600,7 +1600,7 @@
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>2329677</t>
+          <t>2329605</t>
         </is>
       </c>
     </row>
@@ -1647,7 +1647,7 @@
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>20.246</t>
+          <t>20.249</t>
         </is>
       </c>
     </row>

</xml_diff>